<commit_message>
modify request from bureau
</commit_message>
<xml_diff>
--- a/www/assets/xlsx/sur_tracking.tpl.xlsx
+++ b/www/assets/xlsx/sur_tracking.tpl.xlsx
@@ -23,39 +23,48 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>桃園市ＯＯ地政事務所</t>
+    <t>收件年</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收件字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收件號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>複丈原因</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收件日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>複丈日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逾期日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測量員</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>處理情形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>核章欄</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>測量案件管制清冊</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>收件字號</t>
-  </si>
-  <si>
-    <t>收件時間</t>
-  </si>
-  <si>
-    <t>複丈原因</t>
-  </si>
-  <si>
-    <t>辦理情形</t>
-  </si>
-  <si>
-    <t>測量員</t>
-  </si>
-  <si>
-    <t>延期複丈原因</t>
-  </si>
-  <si>
-    <t>複丈時間</t>
-  </si>
-  <si>
-    <t>逾期時間</t>
-  </si>
-  <si>
-    <t>承辦人簽章</t>
   </si>
 </sst>
 </file>
@@ -114,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -137,13 +146,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -156,10 +174,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -466,81 +493,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="8" width="21.75" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.875" style="2" customWidth="1"/>
+    <col min="1" max="3" width="10.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="2" customWidth="1"/>
+    <col min="5" max="7" width="12.625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="30.625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -551,7 +577,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -562,7 +588,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -573,7 +599,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -584,7 +610,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -595,7 +621,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -606,7 +632,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -617,7 +643,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -628,7 +654,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -639,7 +665,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -650,7 +676,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -661,7 +687,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -672,7 +698,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1277,21 +1303,9 @@
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
     </row>
-    <row r="71" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.98425196850393704" top="0.78740157480314965" bottom="0.98425196850393704" header="0.59055118110236215" footer="0.6889763779527559"/>

</xml_diff>